<commit_message>
Hood commands fix column
</commit_message>
<xml_diff>
--- a/Excel/Hood/2022.02.18/02.03.2022 HOOD — загрузка.xlsx
+++ b/Excel/Hood/2022.02.18/02.03.2022 HOOD — загрузка.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2620BBA-5264-4C1A-96D3-66ECAD0D820B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\Hood\2022.02.18\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F48279F-62F6-428E-8D7B-BAB89B092F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CF7BE728-4E5A-484C-A229-5E33F4CC11D4}"/>
   </bookViews>
@@ -57,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="371">
   <si>
     <t>Артикул</t>
   </si>
@@ -1041,6 +1046,135 @@
   </si>
   <si>
     <t>92-001-09-00</t>
+  </si>
+  <si>
+    <t>Jack Murphy</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Deer Valley</t>
+  </si>
+  <si>
+    <t>Queensbridge</t>
+  </si>
+  <si>
+    <t>Hell'S Kitchen</t>
+  </si>
+  <si>
+    <t>Marcy</t>
+  </si>
+  <si>
+    <t>Flatbush</t>
+  </si>
+  <si>
+    <t>Malibu</t>
+  </si>
+  <si>
+    <t>Fairfax</t>
+  </si>
+  <si>
+    <t>Westwood</t>
+  </si>
+  <si>
+    <t>Brentwood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queens </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bronx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koreatown </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compton </t>
+  </si>
+  <si>
+    <t>Venice</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Baltimore</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Happy Valley</t>
+  </si>
+  <si>
+    <t>Kings County</t>
+  </si>
+  <si>
+    <t>Hidden Hills</t>
+  </si>
+  <si>
+    <t>Love Park</t>
+  </si>
+  <si>
+    <t>Coney Island</t>
+  </si>
+  <si>
+    <t>Park Hill</t>
+  </si>
+  <si>
+    <t>Harlem</t>
+  </si>
+  <si>
+    <t>Bed Stuy</t>
+  </si>
+  <si>
+    <t>8 Mile</t>
+  </si>
+  <si>
+    <t>Long Beach</t>
+  </si>
+  <si>
+    <t>Chavez Ravine</t>
+  </si>
+  <si>
+    <t>South Central</t>
+  </si>
+  <si>
+    <t>Compton</t>
+  </si>
+  <si>
+    <t>Bel Air</t>
+  </si>
+  <si>
+    <t>Beverly Hills</t>
+  </si>
+  <si>
+    <t>Команды</t>
   </si>
 </sst>
 </file>
@@ -1510,11 +1644,11 @@
   <sheetPr codeName="Лист28">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W401"/>
+  <dimension ref="A1:X401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO35" sqref="AO35"/>
+      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,7 +1679,7 @@
     <col min="24" max="16384" width="18.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1615,8 +1749,11 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X1" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1686,8 +1823,11 @@
       <c r="W2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1757,8 +1897,11 @@
       <c r="W3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X3" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1828,8 +1971,11 @@
       <c r="W4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X4" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1899,8 +2045,11 @@
       <c r="W5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1970,8 +2119,11 @@
       <c r="W6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X6" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -2041,8 +2193,11 @@
       <c r="W7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X7" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -2112,8 +2267,11 @@
       <c r="W8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X8" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -2183,8 +2341,11 @@
       <c r="W9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -2254,8 +2415,11 @@
       <c r="W10" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -2325,8 +2489,11 @@
       <c r="W11" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X11" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -2396,8 +2563,11 @@
       <c r="W12" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X12" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -2467,8 +2637,11 @@
       <c r="W13" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X13" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -2538,8 +2711,11 @@
       <c r="W14" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X14" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>125</v>
       </c>
@@ -2609,8 +2785,11 @@
       <c r="W15" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X15" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -2680,8 +2859,11 @@
       <c r="W16" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X16" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -2751,8 +2933,11 @@
       <c r="W17" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X17" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -2822,8 +3007,11 @@
       <c r="W18" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X18" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>149</v>
       </c>
@@ -2893,8 +3081,11 @@
       <c r="W19" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X19" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>155</v>
       </c>
@@ -2964,8 +3155,11 @@
       <c r="W20" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X20" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>163</v>
       </c>
@@ -3035,8 +3229,11 @@
       <c r="W21" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X21" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>170</v>
       </c>
@@ -3106,8 +3303,11 @@
       <c r="W22" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X22" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>176</v>
       </c>
@@ -3177,8 +3377,11 @@
       <c r="W23" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X23" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>181</v>
       </c>
@@ -3248,8 +3451,11 @@
       <c r="W24" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X24" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>186</v>
       </c>
@@ -3319,8 +3525,11 @@
       <c r="W25" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X25" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>192</v>
       </c>
@@ -3390,8 +3599,11 @@
       <c r="W26" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X26" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>198</v>
       </c>
@@ -3461,8 +3673,11 @@
       <c r="W27" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X27" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>204</v>
       </c>
@@ -3532,8 +3747,11 @@
       <c r="W28" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X28" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>209</v>
       </c>
@@ -3603,8 +3821,11 @@
       <c r="W29" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X29" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>214</v>
       </c>
@@ -3674,8 +3895,11 @@
       <c r="W30" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X30" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>222</v>
       </c>
@@ -3745,8 +3969,11 @@
       <c r="W31" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X31" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>227</v>
       </c>
@@ -3816,8 +4043,11 @@
       <c r="W32" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X32" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>233</v>
       </c>
@@ -3887,8 +4117,11 @@
       <c r="W33" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X33" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>238</v>
       </c>
@@ -3958,8 +4191,11 @@
       <c r="W34" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X34" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>243</v>
       </c>
@@ -4029,8 +4265,11 @@
       <c r="W35" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X35" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>248</v>
       </c>
@@ -4100,8 +4339,11 @@
       <c r="W36" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X36" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>253</v>
       </c>
@@ -4171,8 +4413,11 @@
       <c r="W37" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X37" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>258</v>
       </c>
@@ -4242,8 +4487,11 @@
       <c r="W38" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X38" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>263</v>
       </c>
@@ -4313,8 +4561,11 @@
       <c r="W39" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X39" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>268</v>
       </c>
@@ -4384,8 +4635,11 @@
       <c r="W40" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X40" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>273</v>
       </c>
@@ -4455,8 +4709,11 @@
       <c r="W41" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X41" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>278</v>
       </c>
@@ -4526,8 +4783,11 @@
       <c r="W42" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X42" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>283</v>
       </c>
@@ -4597,8 +4857,11 @@
       <c r="W43" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X43" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>288</v>
       </c>
@@ -4668,8 +4931,11 @@
       <c r="W44" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X44" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>293</v>
       </c>
@@ -4739,8 +5005,11 @@
       <c r="W45" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X45" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>298</v>
       </c>
@@ -4810,8 +5079,11 @@
       <c r="W46" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X46" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>303</v>
       </c>
@@ -4881,8 +5153,11 @@
       <c r="W47" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X47" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>308</v>
       </c>
@@ -4952,8 +5227,11 @@
       <c r="W48" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X48" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>313</v>
       </c>
@@ -5023,8 +5301,11 @@
       <c r="W49" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X49" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>318</v>
       </c>
@@ -5094,8 +5375,11 @@
       <c r="W50" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X50" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>323</v>
       </c>
@@ -5165,8 +5449,11 @@
       <c r="W51" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X51" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -5191,7 +5478,7 @@
       <c r="V52"/>
       <c r="W52"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -5216,7 +5503,7 @@
       <c r="V53"/>
       <c r="W53"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -5241,7 +5528,7 @@
       <c r="V54"/>
       <c r="W54"/>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -5266,7 +5553,7 @@
       <c r="V55"/>
       <c r="W55"/>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
@@ -5291,7 +5578,7 @@
       <c r="V56"/>
       <c r="W56"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
@@ -5316,7 +5603,7 @@
       <c r="V57"/>
       <c r="W57"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -5341,7 +5628,7 @@
       <c r="V58"/>
       <c r="W58"/>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -5366,7 +5653,7 @@
       <c r="V59"/>
       <c r="W59"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -5391,7 +5678,7 @@
       <c r="V60"/>
       <c r="W60"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -5416,7 +5703,7 @@
       <c r="V61"/>
       <c r="W61"/>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -5441,7 +5728,7 @@
       <c r="V62"/>
       <c r="W62"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -5466,7 +5753,7 @@
       <c r="V63"/>
       <c r="W63"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>

</xml_diff>